<commit_message>
Plotting the Day 3 Data - Farooq
</commit_message>
<xml_diff>
--- a/OtherDaysData/Day3Logsheet.xlsx
+++ b/OtherDaysData/Day3Logsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olanrewaju Farooq\Downloads\MIROceanographyAnalysis\OtherDaysData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D736068-E65C-4267-AC2C-24B84491C5F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9208B9-30CA-4FC7-9532-F48596BBF89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -448,7 +448,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>